<commit_message>
Added extent reports and implemented some of the OOPS concepts
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Testdata.xlsx
+++ b/src/test/resources/excel/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Polaris Office Sheet" lastEdited="6" lowestEdited="6" rupBuild="9.101.23.39576"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="550" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="userNamePage" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1062,7 +1062,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.000000"/>
@@ -1113,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.000000"/>
@@ -1127,14 +1127,13 @@
     <col min="4" max="4" width="13.14785753" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="D1" s="0" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3"/>
-      <c r="D2" s="0" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" s="0" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>